<commit_message>
fix: modification of the Excel files in public
</commit_message>
<xml_diff>
--- a/public/excel/Voeux.xlsx
+++ b/public/excel/Voeux.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="251">
   <si>
     <t xml:space="preserve">BUT S1</t>
   </si>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">PPP - Eric Bittar</t>
   </si>
   <si>
-    <t xml:space="preserve"> PPP</t>
+    <t xml:space="preserve">PPP</t>
   </si>
   <si>
     <t xml:space="preserve">PPP - Valérie Chevalarias</t>
@@ -344,9 +344,6 @@
   </si>
   <si>
     <t xml:space="preserve">MR214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPP</t>
   </si>
   <si>
     <t xml:space="preserve">PPP - Ludovic Lambert</t>
@@ -2135,10 +2132,10 @@
   <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
@@ -3862,7 +3859,7 @@
       <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.04"/>
@@ -5676,7 +5673,7 @@
       </c>
       <c r="F32" s="73"/>
       <c r="G32" s="73" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="H32" s="15"/>
       <c r="I32" s="15" t="n">
@@ -5748,7 +5745,7 @@
         <v>88</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="35" t="n">
         <v>1</v>
@@ -5832,7 +5829,7 @@
         <v>88</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="13" t="n">
         <v>4</v>
@@ -5938,7 +5935,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -6018,7 +6015,7 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
@@ -6029,7 +6026,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="105.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="74" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="2" t="s">
@@ -6113,10 +6110,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="75" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>1</v>
@@ -6130,7 +6127,7 @@
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H2" s="15" t="n">
         <v>1</v>
@@ -6221,10 +6218,10 @@
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="28" t="n">
         <v>8</v>
@@ -6277,10 +6274,10 @@
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>99</v>
       </c>
       <c r="C5" s="12" t="n">
         <v>8</v>
@@ -6294,7 +6291,7 @@
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -6333,10 +6330,10 @@
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="77" t="s">
         <v>101</v>
-      </c>
-      <c r="B6" s="77" t="s">
-        <v>102</v>
       </c>
       <c r="C6" s="28" t="n">
         <v>1</v>
@@ -6350,7 +6347,7 @@
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
@@ -6390,7 +6387,7 @@
     <row r="7" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="76"/>
       <c r="B7" s="77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="28" t="n">
         <v>2</v>
@@ -6404,7 +6401,7 @@
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
@@ -6444,7 +6441,7 @@
     <row r="8" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="76"/>
       <c r="B8" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="28" t="n">
         <v>1</v>
@@ -6458,7 +6455,7 @@
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
@@ -6497,10 +6494,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>108</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>109</v>
       </c>
       <c r="C9" s="12" t="n">
         <v>1</v>
@@ -6599,10 +6596,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>110</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>111</v>
       </c>
       <c r="C11" s="28" t="n">
         <v>1</v>
@@ -6616,7 +6613,7 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H11" s="27" t="n">
         <v>1</v>
@@ -6706,7 +6703,7 @@
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="76"/>
       <c r="B13" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="28" t="n">
         <v>2</v>
@@ -6720,7 +6717,7 @@
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H13" s="27" t="n">
         <v>1</v>
@@ -6810,7 +6807,7 @@
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="76"/>
       <c r="B15" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" s="28" t="n">
         <v>1</v>
@@ -6824,7 +6821,7 @@
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H15" s="27" t="n">
         <v>1</v>
@@ -6913,10 +6910,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>118</v>
       </c>
       <c r="C17" s="12" t="n">
         <v>1</v>
@@ -6930,7 +6927,7 @@
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -6970,7 +6967,7 @@
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="75"/>
       <c r="B18" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="12" t="n">
         <v>2</v>
@@ -6984,7 +6981,7 @@
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
@@ -7024,7 +7021,7 @@
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="75"/>
       <c r="B19" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="12" t="n">
         <v>1</v>
@@ -7038,7 +7035,7 @@
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
@@ -7077,10 +7074,10 @@
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>124</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>125</v>
       </c>
       <c r="C20" s="28" t="n">
         <v>1</v>
@@ -7173,10 +7170,10 @@
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>127</v>
       </c>
       <c r="C22" s="22" t="n">
         <v>1</v>
@@ -7273,10 +7270,10 @@
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="76" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="27" t="s">
         <v>128</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>129</v>
       </c>
       <c r="C24" s="28" t="n">
         <v>1</v>
@@ -7427,10 +7424,10 @@
     </row>
     <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="75" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>131</v>
       </c>
       <c r="C27" s="12" t="n">
         <v>4</v>
@@ -7485,10 +7482,10 @@
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="27" t="s">
         <v>132</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>133</v>
       </c>
       <c r="C28" s="28" t="n">
         <v>1</v>
@@ -7587,10 +7584,10 @@
     </row>
     <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="75" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C30" s="12" t="n">
         <v>1</v>
@@ -7695,7 +7692,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>85</v>
@@ -7803,7 +7800,7 @@
     </row>
     <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="75" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>45</v>
@@ -7875,7 +7872,7 @@
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>47</v>
@@ -7947,10 +7944,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B36" s="78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="79" t="n">
         <v>4</v>
@@ -7964,7 +7961,7 @@
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="20" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="H36" s="15" t="n">
         <v>1</v>
@@ -8006,7 +8003,7 @@
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="75"/>
       <c r="B37" s="78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C37" s="13" t="n">
         <v>4</v>
@@ -8116,7 +8113,7 @@
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.66"/>
@@ -8127,7 +8124,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="105.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="82" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="82"/>
       <c r="C1" s="2" t="s">
@@ -8190,10 +8187,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>140</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>141</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>1</v>
@@ -8207,7 +8204,7 @@
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
@@ -8227,7 +8224,7 @@
         <v>3</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P2" s="15" t="n">
         <v>3</v>
@@ -8249,7 +8246,7 @@
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="83"/>
       <c r="B3" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="12" t="n">
         <v>1</v>
@@ -8263,7 +8260,7 @@
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="15"/>
@@ -8300,7 +8297,7 @@
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="83"/>
       <c r="B4" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="12" t="n">
         <v>2</v>
@@ -8314,7 +8311,7 @@
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="15" t="n">
@@ -8342,7 +8339,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="12" t="n">
@@ -8385,10 +8382,10 @@
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>148</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>149</v>
       </c>
       <c r="C6" s="28" t="n">
         <v>8</v>
@@ -8401,10 +8398,10 @@
         <v>36</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>151</v>
       </c>
       <c r="H6" s="31"/>
       <c r="I6" s="27"/>
@@ -8440,10 +8437,10 @@
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="84" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>153</v>
       </c>
       <c r="C7" s="12" t="n">
         <v>8</v>
@@ -8456,10 +8453,10 @@
         <v>27</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="15"/>
@@ -8495,10 +8492,10 @@
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="85" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>155</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>156</v>
       </c>
       <c r="C8" s="28" t="n">
         <v>1</v>
@@ -8512,7 +8509,7 @@
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H8" s="31"/>
       <c r="I8" s="27"/>
@@ -8549,7 +8546,7 @@
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="85"/>
       <c r="B9" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="28" t="n">
         <v>2</v>
@@ -8563,7 +8560,7 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H9" s="31"/>
       <c r="I9" s="27"/>
@@ -8599,10 +8596,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" s="12" t="n">
         <v>2</v>
@@ -8616,7 +8613,7 @@
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="15"/>
@@ -8652,10 +8649,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="84" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="12" t="n">
         <v>2</v>
@@ -8669,7 +8666,7 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="15"/>
@@ -8699,7 +8696,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="12" t="n">
@@ -8742,10 +8739,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="85" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>164</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>165</v>
       </c>
       <c r="C13" s="28" t="n">
         <v>1</v>
@@ -8758,10 +8755,10 @@
         <v>27</v>
       </c>
       <c r="F13" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13" s="20" t="s">
         <v>166</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>167</v>
       </c>
       <c r="H13" s="31"/>
       <c r="I13" s="27"/>
@@ -8797,10 +8794,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="84" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>169</v>
       </c>
       <c r="C14" s="12" t="n">
         <v>2</v>
@@ -8813,10 +8810,10 @@
         <v>18</v>
       </c>
       <c r="F14" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>166</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>167</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="15"/>
@@ -8852,10 +8849,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="85" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>170</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>171</v>
       </c>
       <c r="C15" s="28" t="n">
         <v>1</v>
@@ -8869,7 +8866,7 @@
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H15" s="31"/>
       <c r="I15" s="27" t="n">
@@ -8942,10 +8939,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="86" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>173</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>174</v>
       </c>
       <c r="C17" s="22" t="n">
         <v>1</v>
@@ -8959,7 +8956,7 @@
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H17" s="25"/>
       <c r="I17" s="23"/>
@@ -9026,10 +9023,10 @@
     </row>
     <row r="19" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="85" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>176</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>177</v>
       </c>
       <c r="C19" s="28" t="n">
         <v>4</v>
@@ -9043,7 +9040,7 @@
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H19" s="31"/>
       <c r="I19" s="27"/>
@@ -9079,10 +9076,10 @@
     </row>
     <row r="20" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="84" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>179</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>180</v>
       </c>
       <c r="C20" s="12" t="n">
         <v>4</v>
@@ -9132,10 +9129,10 @@
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="87" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>181</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>182</v>
       </c>
       <c r="C21" s="28" t="n">
         <v>4</v>
@@ -9185,7 +9182,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="84" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>45</v>
@@ -9238,7 +9235,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="85" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>47</v>
@@ -9338,10 +9335,10 @@
     </row>
     <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="84" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="C25" s="12" t="n">
         <v>4</v>
@@ -9357,7 +9354,7 @@
         <v>52</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="15"/>
@@ -9442,7 +9439,7 @@
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.15"/>
@@ -9453,7 +9450,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="105.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="88" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="88"/>
       <c r="C1" s="89" t="s">
@@ -9531,10 +9528,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="94" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>188</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>3</v>
@@ -9560,7 +9557,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="95" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L2" s="95"/>
       <c r="M2" s="15" t="n">
@@ -9570,10 +9567,10 @@
         <v>3</v>
       </c>
       <c r="O2" s="95" t="s">
+        <v>188</v>
+      </c>
+      <c r="P2" s="96" t="s">
         <v>189</v>
-      </c>
-      <c r="P2" s="96" t="s">
-        <v>190</v>
       </c>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
@@ -9583,16 +9580,16 @@
       <c r="V2" s="16"/>
       <c r="W2" s="15"/>
       <c r="X2" s="96" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Y2" s="96"/>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="99" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="C3" s="28" t="n">
         <v>3</v>
@@ -9606,7 +9603,7 @@
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="H3" s="27" t="n">
         <v>1</v>
@@ -9649,7 +9646,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="94" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>47</v>
@@ -9713,7 +9710,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="99" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>45</v>
@@ -9777,7 +9774,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="94" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>42</v>
@@ -9818,7 +9815,7 @@
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
       <c r="S6" s="103" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T6" s="103"/>
       <c r="U6" s="15"/>
@@ -9873,10 +9870,10 @@
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="99" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C8" s="28" t="n">
         <v>3</v>
@@ -9890,7 +9887,7 @@
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
@@ -9923,10 +9920,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="94" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>197</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>198</v>
       </c>
       <c r="C9" s="12" t="n">
         <v>3</v>
@@ -9983,10 +9980,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="99" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>199</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>200</v>
       </c>
       <c r="C10" s="28" t="n">
         <v>1</v>
@@ -10000,7 +9997,7 @@
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H10" s="27" t="n">
         <v>1</v>
@@ -10097,10 +10094,10 @@
     </row>
     <row r="12" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="104" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="44" t="s">
         <v>202</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>203</v>
       </c>
       <c r="C12" s="12" t="n">
         <v>3</v>
@@ -10114,7 +10111,7 @@
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H12" s="15" t="n">
         <v>4</v>
@@ -10157,10 +10154,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="105" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13" s="63" t="s">
         <v>205</v>
-      </c>
-      <c r="B13" s="63" t="s">
-        <v>206</v>
       </c>
       <c r="C13" s="28" t="n">
         <v>1</v>
@@ -10174,7 +10171,7 @@
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
@@ -10251,10 +10248,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="106" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="107" t="s">
         <v>208</v>
-      </c>
-      <c r="B15" s="107" t="s">
-        <v>209</v>
       </c>
       <c r="C15" s="108" t="n">
         <v>5</v>
@@ -10268,7 +10265,7 @@
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H15" s="107" t="n">
         <v>4</v>
@@ -10311,10 +10308,10 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="114" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="115" t="s">
         <v>211</v>
-      </c>
-      <c r="B16" s="115" t="s">
-        <v>212</v>
       </c>
       <c r="C16" s="116" t="n">
         <v>3</v>
@@ -10327,10 +10324,10 @@
         <v>15</v>
       </c>
       <c r="F16" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>213</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>214</v>
       </c>
       <c r="H16" s="115" t="n">
         <v>3</v>
@@ -10364,7 +10361,7 @@
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="114"/>
       <c r="B17" s="115" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C17" s="116" t="n">
         <v>3</v>
@@ -10378,7 +10375,7 @@
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H17" s="115"/>
       <c r="I17" s="115"/>
@@ -10411,10 +10408,10 @@
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="106" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18" s="107" t="s">
         <v>217</v>
-      </c>
-      <c r="B18" s="107" t="s">
-        <v>218</v>
       </c>
       <c r="C18" s="108" t="n">
         <v>2</v>
@@ -10427,10 +10424,10 @@
         <v>22</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H18" s="107"/>
       <c r="I18" s="107"/>
@@ -10463,10 +10460,10 @@
     </row>
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="119" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" s="120" t="s">
         <v>220</v>
-      </c>
-      <c r="B19" s="120" t="s">
-        <v>221</v>
       </c>
       <c r="C19" s="121" t="n">
         <v>1</v>
@@ -10513,10 +10510,10 @@
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="127" t="s">
+        <v>221</v>
+      </c>
+      <c r="B20" s="128" t="s">
         <v>222</v>
-      </c>
-      <c r="B20" s="128" t="s">
-        <v>223</v>
       </c>
       <c r="C20" s="129" t="n">
         <v>1</v>
@@ -10561,10 +10558,10 @@
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="119" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" s="120" t="s">
         <v>224</v>
-      </c>
-      <c r="B21" s="120" t="s">
-        <v>225</v>
       </c>
       <c r="C21" s="121" t="n">
         <v>1</v>
@@ -10578,7 +10575,7 @@
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H21" s="120"/>
       <c r="I21" s="120"/>
@@ -10611,10 +10608,10 @@
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="127" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" s="128" t="s">
         <v>227</v>
-      </c>
-      <c r="B22" s="128" t="s">
-        <v>228</v>
       </c>
       <c r="C22" s="129" t="n">
         <v>1</v>
@@ -10627,10 +10624,10 @@
         <v>20</v>
       </c>
       <c r="F22" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" s="20" t="s">
         <v>229</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>230</v>
       </c>
       <c r="H22" s="128" t="n">
         <v>4</v>
@@ -10663,10 +10660,10 @@
     </row>
     <row r="23" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="133" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" s="120" t="s">
         <v>231</v>
-      </c>
-      <c r="B23" s="120" t="s">
-        <v>232</v>
       </c>
       <c r="C23" s="121" t="n">
         <v>1</v>
@@ -10679,10 +10676,10 @@
         <v>22</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H23" s="120"/>
       <c r="I23" s="120"/>
@@ -10764,7 +10761,7 @@
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.39"/>
@@ -10779,7 +10776,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="105.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="138" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B1" s="138"/>
       <c r="C1" s="2" t="s">
@@ -10872,10 +10869,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="140" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>234</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>235</v>
       </c>
       <c r="C2" s="12" t="n">
         <v>1</v>
@@ -10892,7 +10889,7 @@
         <v>83</v>
       </c>
       <c r="H2" s="141" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I2" s="141"/>
       <c r="J2" s="141"/>
@@ -10908,7 +10905,7 @@
       <c r="T2" s="141"/>
       <c r="U2" s="141"/>
       <c r="V2" s="142" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="W2" s="142"/>
       <c r="X2" s="142"/>
@@ -10976,7 +10973,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="144" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>85</v>
@@ -11076,7 +11073,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="140" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>47</v>
@@ -11129,10 +11126,10 @@
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="144" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="C7" s="28" t="n">
         <v>3</v>
@@ -11148,7 +11145,7 @@
         <v>52</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="H7" s="141"/>
       <c r="I7" s="141"/>
@@ -11184,7 +11181,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="140" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>45</v>
@@ -11237,10 +11234,10 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="145" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="115" t="s">
         <v>242</v>
-      </c>
-      <c r="B9" s="115" t="s">
-        <v>243</v>
       </c>
       <c r="C9" s="116" t="n">
         <v>5</v>
@@ -11254,7 +11251,7 @@
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H9" s="141"/>
       <c r="I9" s="141"/>
@@ -11290,10 +11287,10 @@
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="147" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="107" t="s">
         <v>245</v>
-      </c>
-      <c r="B10" s="107" t="s">
-        <v>246</v>
       </c>
       <c r="C10" s="108" t="n">
         <v>3</v>
@@ -11306,10 +11303,10 @@
         <v>20</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H10" s="141"/>
       <c r="I10" s="141"/>
@@ -11345,10 +11342,10 @@
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="120" t="s">
         <v>248</v>
-      </c>
-      <c r="B11" s="120" t="s">
-        <v>249</v>
       </c>
       <c r="C11" s="121" t="n">
         <v>1</v>
@@ -11361,7 +11358,7 @@
         <v>24</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>31</v>
@@ -11400,10 +11397,10 @@
     </row>
     <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="151" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B12" s="128" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C12" s="129" t="n">
         <v>1</v>
@@ -11417,7 +11414,7 @@
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H12" s="141"/>
       <c r="I12" s="141"/>
@@ -11453,10 +11450,10 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="149" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B13" s="120" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C13" s="121" t="n">
         <v>1</v>
@@ -11470,7 +11467,7 @@
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H13" s="141"/>
       <c r="I13" s="141"/>

</xml_diff>

<commit_message>
fix: update for the excel files
</commit_message>
<xml_diff>
--- a/public/excel/Voeux.xlsx
+++ b/public/excel/Voeux.xlsx
@@ -2129,13 +2129,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB32"/>
+  <dimension ref="A1:AB38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
@@ -3794,6 +3794,24 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="0" t="e">
+        <f aca="false">counta(H2:Z30)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="0" t="n">
+        <f aca="false">(G38+S2!G39+S3!G40+S4!G28+S5!G27+S6!G33)</f>
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="0" t="n">
+        <f aca="false">COUNTA(H2:O30,Q2:W30,Z2:Z30)</f>
+        <v>222</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="35">
@@ -3856,10 +3874,10 @@
   <dimension ref="A1:AD39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
+      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.04"/>
@@ -5936,6 +5954,9 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>91</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -6009,13 +6030,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB38"/>
+  <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
@@ -8043,6 +8064,12 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="0" t="n">
+        <f aca="false">COUNTA(H2:O37,Q2:W37,Z2:AA37)</f>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -8107,13 +8134,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.66"/>
@@ -9391,6 +9418,12 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="0" t="n">
+        <f aca="false">COUNTA(H2:N25,P2:T25)</f>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -9433,13 +9466,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.15"/>
@@ -10713,6 +10746,12 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="0" t="n">
+        <f aca="false">COUNTA(H2:J23,K2:O23,Q2:W23)</f>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -10758,10 +10797,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.39"/>
@@ -12041,7 +12080,10 @@
       <c r="D33" s="163"/>
       <c r="E33" s="163"/>
       <c r="F33" s="163"/>
-      <c r="G33" s="163"/>
+      <c r="G33" s="163" t="n">
+        <f aca="false">COUNTA(Z2:AD13)</f>
+        <v>48</v>
+      </c>
       <c r="H33" s="163"/>
       <c r="I33" s="163"/>
       <c r="J33" s="163"/>

</xml_diff>

<commit_message>
fix: correct french spelling errors in Excel file
</commit_message>
<xml_diff>
--- a/public/excel/Voeux.xlsx
+++ b/public/excel/Voeux.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="S1" sheetId="1" state="visible" r:id="rId2"/>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">CM</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / Python / Algo</t>
+    <t xml:space="preserve">Développement / Python / Algo</t>
   </si>
   <si>
     <t xml:space="preserve">Vacances de la Toussaint</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">TDM</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / HTML / CSS / Web</t>
+    <t xml:space="preserve">Développement / HTML / CSS / Web</t>
   </si>
   <si>
     <t xml:space="preserve">MR103</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Codages</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / Binaire / Maths</t>
+    <t xml:space="preserve">Développement / Binaire / Maths</t>
   </si>
   <si>
     <t xml:space="preserve">MR104</t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">Programmation orientée objets (PHP)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / PHP / POO</t>
+    <t xml:space="preserve">Développement / PHP / POO</t>
   </si>
   <si>
     <t xml:space="preserve">Vacances d’hiver</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">Web (PHP, CRUD)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / PHP / Web</t>
+    <t xml:space="preserve">Développement / PHP / Web</t>
   </si>
   <si>
     <t xml:space="preserve">MR203-MR205</t>
@@ -412,19 +412,19 @@
     <t xml:space="preserve">Langage pour la POO (C++)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / C++</t>
+    <t xml:space="preserve">Développement / C++</t>
   </si>
   <si>
     <t xml:space="preserve">Langage pour la POO (C#)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / C#</t>
+    <t xml:space="preserve">Développement / C#</t>
   </si>
   <si>
     <t xml:space="preserve">Langage pour la POO (Python)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / Python</t>
+    <t xml:space="preserve">Développement / Python</t>
   </si>
   <si>
     <t xml:space="preserve">MR305</t>
@@ -508,13 +508,13 @@
     <t xml:space="preserve">Flask</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / Python / Web</t>
+    <t xml:space="preserve">Développement / Python / Web</t>
   </si>
   <si>
     <t xml:space="preserve">ASP .NET</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / C# / Web</t>
+    <t xml:space="preserve">Développement / C# / Web</t>
   </si>
   <si>
     <t xml:space="preserve">MR413R</t>
@@ -529,7 +529,7 @@
     <t xml:space="preserve">1R</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / Symfony / Tests</t>
+    <t xml:space="preserve">Développement / Symfony / Tests</t>
   </si>
   <si>
     <t xml:space="preserve">MR410</t>
@@ -538,7 +538,7 @@
     <t xml:space="preserve">Complément web (React)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / JavaScript / Web / React</t>
+    <t xml:space="preserve">Développement / JavaScript / Web / React</t>
   </si>
   <si>
     <t xml:space="preserve">MR411R</t>
@@ -547,25 +547,25 @@
     <t xml:space="preserve">Développement mobile (Flutter)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / Mobile / Flutter / Dart</t>
+    <t xml:space="preserve">Développement / Mobile / Flutter / Dart</t>
   </si>
   <si>
     <t xml:space="preserve">Développement mobile (MAUI)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / Mobile / MAUI / C#</t>
+    <t xml:space="preserve">Développement / Mobile / MAUI / C#</t>
   </si>
   <si>
     <t xml:space="preserve">Complément technologique (Réalité virtuelle / réalité augmentée)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / VR-RA / C++ / C#</t>
+    <t xml:space="preserve">Développement / VR-RA / C++ / C#</t>
   </si>
   <si>
     <t xml:space="preserve">Complément technologique (Conception des systèmes automatisés)</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / C# / Scratch</t>
+    <t xml:space="preserve">Développement / C# / Scratch</t>
   </si>
   <si>
     <t xml:space="preserve">MR410A</t>
@@ -757,7 +757,7 @@
     <t xml:space="preserve">Techniques d'IA</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement / Python / IA</t>
+    <t xml:space="preserve">Développement / Python / IA</t>
   </si>
   <si>
     <t xml:space="preserve">MR511A</t>
@@ -822,7 +822,7 @@
     <t xml:space="preserve">Maintenance applicative</t>
   </si>
   <si>
-    <t xml:space="preserve">Dévéloppement</t>
+    <t xml:space="preserve">Développement</t>
   </si>
   <si>
     <t xml:space="preserve">MR605A</t>
@@ -2131,11 +2131,11 @@
   </sheetPr>
   <dimension ref="A1:AB38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
@@ -3796,9 +3796,9 @@
       <c r="A32" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G36" s="0" t="e">
-        <f aca="false">counta(H2:Z30)</f>
-        <v>#NAME?</v>
+      <c r="G36" s="0" t="n">
+        <f aca="false">COUNTA(H2:Z30)</f>
+        <v>224</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3874,10 +3874,10 @@
   <dimension ref="A1:AD39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.04"/>
@@ -6033,10 +6033,10 @@
   <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
@@ -8137,10 +8137,10 @@
   <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.66"/>
@@ -9469,10 +9469,10 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.15"/>
@@ -10796,11 +10796,11 @@
   </sheetPr>
   <dimension ref="A1:AE55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.39"/>

</xml_diff>